<commit_message>
Eh git hub mapa conceptual del guion 7 de grado 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/ESCALETA_LE_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/ESCALETA_LE_06_04_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\GITHUB2015\Lenguaje\fuentes\contenidos\grado06\guion04\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -1217,34 +1222,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1284,6 +1271,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1346,7 +1351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1381,7 +1386,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1592,9 +1597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P41" sqref="P41"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,94 +1627,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="31" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="R1" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="48" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="46"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5248,6 +5253,12 @@
     <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5262,12 +5273,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>